<commit_message>
ajustes de vistas responsive y pequeñas mejoras en filtros, ajuste tabla
</commit_message>
<xml_diff>
--- a/data/ventas.xlsx
+++ b/data/ventas.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1253,9 +1253,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>V-1770952993547</v>
+      </c>
+      <c r="B38" t="str">
+        <v>12/2/2026</v>
+      </c>
+      <c r="C38" t="str">
+        <v>10:23 p. m.</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Stiven</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Aguardiente Amarillo Caja (x1)</v>
+      </c>
+      <c r="F38">
+        <v>122000</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G37"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G38"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>